<commit_message>
Updates & upgrades Python
</commit_message>
<xml_diff>
--- a/05_xlsx_docx_pdf/distritos-ejemplo_v2.xlsx
+++ b/05_xlsx_docx_pdf/distritos-ejemplo_v2.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Distrito_población" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nueva pestaña" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nueva pestaña1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -393,8 +394,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -491,4 +492,22 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>